<commit_message>
adding new dataset files
</commit_message>
<xml_diff>
--- a/Data/dataset.xlsx
+++ b/Data/dataset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nilesh\OneDrive - MethodHub Software Private Limited\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAMEER\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D87644C-3DFC-476D-BC26-7EFE5643EB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
   <si>
     <t>RecipeId</t>
   </si>
@@ -557,12 +558,366 @@
   <si>
     <t>Healthy Heart Bowl</t>
   </si>
+  <si>
+    <t>Jeevan (J)</t>
+  </si>
+  <si>
+    <t>c("Ashguard","Cucmber","Lemon")</t>
+  </si>
+  <si>
+    <t>Amrit (A)</t>
+  </si>
+  <si>
+    <t>Tript (T)</t>
+  </si>
+  <si>
+    <t>Sanjevani (S)</t>
+  </si>
+  <si>
+    <t>Saundrya (S)</t>
+  </si>
+  <si>
+    <t>Ujra (U)</t>
+  </si>
+  <si>
+    <t>c("apple","beetroot","carrot")</t>
+  </si>
+  <si>
+    <t>c("Mosambi","Pineapple","Ginger","Lemon")</t>
+  </si>
+  <si>
+    <t>c("Watermelon","Apple","Mint Leave")</t>
+  </si>
+  <si>
+    <t>c("Orange","Carrot","Lemon")</t>
+  </si>
+  <si>
+    <t>Watermelon, apple, and mint leaf juice offers hydration, antioxidants, and digestive support, promoting overall health in a refreshing, flavorful blend.</t>
+  </si>
+  <si>
+    <t>Orange, carrot, and lemon juice offer a potent mix of vitamin C, antioxidants, and fiber, supporting immunity, skin health, and digestion.</t>
+  </si>
+  <si>
+    <t>Spinach, cucumber, parsley, coconut water, and lemon juice blend provides hydration, antioxidants, and nutrients for overall health and digestion in a refreshing drink.</t>
+  </si>
+  <si>
+    <t>c("Spinach","Cucumber","Parsley","Coconut Water","Lemon")</t>
+  </si>
+  <si>
+    <t>Bottle Guard Juice (B)</t>
+  </si>
+  <si>
+    <t>Spinach  Juice (S)</t>
+  </si>
+  <si>
+    <t>Carrot Juice ( C )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cucumber Juice ( C) </t>
+  </si>
+  <si>
+    <t>Tomato Juice (T)</t>
+  </si>
+  <si>
+    <t>Cabbage Juice ( C )</t>
+  </si>
+  <si>
+    <t>c("Spinach")</t>
+  </si>
+  <si>
+    <t>c("Carrot")</t>
+  </si>
+  <si>
+    <t>c("Bottle Guard")</t>
+  </si>
+  <si>
+    <t>c("Cucumber")</t>
+  </si>
+  <si>
+    <t>c("Tomato")</t>
+  </si>
+  <si>
+    <t>c("Cabbage")</t>
+  </si>
+  <si>
+    <t>Spinach and water offer hydration and essential nutrients, promoting overall health and vitality in a refreshing, low-calorie blend.</t>
+  </si>
+  <si>
+    <t>Carrot and water provide hydration and essential nutrients, promoting eye health, immunity, and digestion in a refreshing, low-calorie drink.</t>
+  </si>
+  <si>
+    <t>Bottle gourd and water blend offers hydration and a low-calorie source of vitamins, minerals, and fiber, promoting digestion and overall health in a refreshing beverage.</t>
+  </si>
+  <si>
+    <t>Cucumber and water provide hydration and essential nutrients, supporting overall health in a refreshing, low-calorie beverage.</t>
+  </si>
+  <si>
+    <t>Tomato and water blend offers hydration and a rich source of vitamins, minerals, and antioxidants, supporting heart health and immune function in a refreshing, low-calorie beverage.</t>
+  </si>
+  <si>
+    <t>Cabbage and water blend offers hydration and a low-calorie source of fiber, vitamins, and antioxidants, supporting digestion and immune health in a refreshing beverage.</t>
+  </si>
+  <si>
+    <t>Bitter Guard Juice ( B)</t>
+  </si>
+  <si>
+    <t>Bitter gourd and cucumber juice offers hydration and a nutrient-rich blend of vitamins, minerals, and antioxidants, supporting digestion and immune health in a refreshing beverage.</t>
+  </si>
+  <si>
+    <t>Apple, beetroot, and carrot juice blend offers a powerhouse of antioxidants, vitamins, and minerals, promoting heart health, digestion, and immune function in a delicious and nutritious beverage.</t>
+  </si>
+  <si>
+    <t>Mosambi, pineapple, ginger, and lemon juice blend offers a refreshing and immune-boosting concoction rich in vitamin C, antioxidants, and digestive aids, supporting overall health and vitality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ash gourd, cucumber, and lemon juice offer hydration and essential nutrients, aiding digestion and promoting overall health in a refreshing, low-calorie blend. </t>
+  </si>
+  <si>
+    <t>Brain Booster (B)</t>
+  </si>
+  <si>
+    <t>Healthy Heart (H)</t>
+  </si>
+  <si>
+    <t>Purify Blood (P)</t>
+  </si>
+  <si>
+    <t>Glow Skin (G)</t>
+  </si>
+  <si>
+    <t>Detox (D)</t>
+  </si>
+  <si>
+    <t>Overnight Oats With Apple (A)</t>
+  </si>
+  <si>
+    <t>Overnight Oats With Few diced Grapes (G)</t>
+  </si>
+  <si>
+    <t>Overnight Oats With Mango and banana (M)</t>
+  </si>
+  <si>
+    <t>Overnight Oats With Kiwi and Banana (K)</t>
+  </si>
+  <si>
+    <t>Overnight Oats With Sapodilla  (S)</t>
+  </si>
+  <si>
+    <t>Overnight Oats With Banana (B)</t>
+  </si>
+  <si>
+    <t>Classic Chickpeas Salad ( C)</t>
+  </si>
+  <si>
+    <t>Garden Harvest Salad (G)</t>
+  </si>
+  <si>
+    <t>Thai Cucumber Salad (T)</t>
+  </si>
+  <si>
+    <t>Ruby Red Salad (R)</t>
+  </si>
+  <si>
+    <t>Sprouts Salad (S)</t>
+  </si>
+  <si>
+    <t>Saute Veggies (S)</t>
+  </si>
+  <si>
+    <t>Brocclie Beetroot Tikki (B)</t>
+  </si>
+  <si>
+    <t>Summer Delight Salad (S)</t>
+  </si>
+  <si>
+    <t>Tropical Green Smoothie (T)</t>
+  </si>
+  <si>
+    <t>Peanut Butter Smoothie (P)</t>
+  </si>
+  <si>
+    <t>Mango Pineapple Smoothie (M)</t>
+  </si>
+  <si>
+    <t>Spinach Smoothie (S)</t>
+  </si>
+  <si>
+    <t>Beetroot Smoothie (B)</t>
+  </si>
+  <si>
+    <t>Mango Smoothie (M)</t>
+  </si>
+  <si>
+    <t>c("Pomogranate","Orange","banana","chikoo","Apple","Grapes")</t>
+  </si>
+  <si>
+    <t>c("Papaya","Pomogranate","Orange","watermelon","Grapes","Chikoo")</t>
+  </si>
+  <si>
+    <t>c("Watermelon","Pomogranate","Pineapple","Avacado"," Orange")</t>
+  </si>
+  <si>
+    <t>This chickpea salad with paneer offers protein, fiber, and essential nutrients that support digestion, heart health, and bone strength, making it a nutritious and satisfying choice for overall well-being.</t>
+  </si>
+  <si>
+    <t>A Ruby Red Salad offers a range of health benefits, including nutrient density, heart health support, digestive health, hydration, weight management aid, blood sugar control, and potential skin health improvements, thanks to its rich array of colorful and nutritious ingredients.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Garden Fresh Protein Salad offers a nutrient-dense meal option that supports muscle maintenance, weight management, heart health, blood sugar control, digestive health, sustained energy, and skin and hair health.</t>
+  </si>
+  <si>
+    <t>This smoothie blend of spinach, banana, mango, and pineapple provides a burst of essential nutrients and antioxidants, promoting vitality and immune support in just one refreshing sip.</t>
+  </si>
+  <si>
+    <t>This smoothie is a nutrient powerhouse, offering sustained energy, heart-healthy fats, and digestive support in a delicious blend of peanut butter, banana, and oat milk.</t>
+  </si>
+  <si>
+    <t>This vibrant smoothie offers tropical flavors and hydrating coconut water, providing a refreshing burst of vitamins, minerals, and hydration for overall wellness and vitality.</t>
+  </si>
+  <si>
+    <t>This smoothie combines spinach, oats milk, and kiwi for a quick and nourishing source of vitamins, minerals, and fiber, promoting overall health and vitality in a refreshing sip.</t>
+  </si>
+  <si>
+    <t>This vibrant smoothie blend of beetroot, milk, and apple offers a nourishing mix of vitamins, minerals, and antioxidants, supporting overall health, digestion, and providing a refreshing energy boost.</t>
+  </si>
+  <si>
+    <t>This creamy smoothie blend of mango, milk, and banana provides a delicious source of vitamins, minerals, and protein, supporting energy levels, immune health, and muscle recovery.</t>
+  </si>
+  <si>
+    <t>c("Pomogranate"," Watermelon","Grapes","Papaya"," Apple","Kiwi")</t>
+  </si>
+  <si>
+    <t>c("Pomogranate","Orange","Banana","Papaya"," Apple"," Kiwi")</t>
+  </si>
+  <si>
+    <t>c("Bitter Guard",Cucumber")</t>
+  </si>
+  <si>
+    <t>c("Spinach","Banana","Mango","Pineapple")</t>
+  </si>
+  <si>
+    <t>c("Peanut butter,"Banana","oats milk")</t>
+  </si>
+  <si>
+    <t>c("Mango","Pineapple","Banana","Coconut Water")</t>
+  </si>
+  <si>
+    <t>c("Spinach","Oats Milk","Kiwi")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("Beetroot","Milk","Apple") </t>
+  </si>
+  <si>
+    <t>c("Mango","Milk","Banana")</t>
+  </si>
+  <si>
+    <t>c("chickpeas","sweet corn","cucumber","carrot","radish","coriander","leaf","paneer")</t>
+  </si>
+  <si>
+    <t>c("beet root","cucumber","carrot","radish","paneer","coriander leaf")</t>
+  </si>
+  <si>
+    <t>c("sprouts","onion","cucumber","radish","carrot","lemon","lettuce")</t>
+  </si>
+  <si>
+    <t>c("broccoli","cucumber","carrot","radish","lettuce"," sweet corn")</t>
+  </si>
+  <si>
+    <t>c("Broccoli","Beetroot","Potato","Ginger","Coriander"Lemon")</t>
+  </si>
+  <si>
+    <t>c("peaches","tomatoes","mango","cilantro",minced")</t>
+  </si>
+  <si>
+    <t>Thai Cucumber Salad is hydrating, low in calories, and rich in nutrients like vitamins and minerals. It provides fiber for digestion, antioxidants for health, and refreshes with its light, flavorful profile.</t>
+  </si>
+  <si>
+    <t>Sprouts salad is a nutrient-packed dish that aids in weight management, digestion, and overall health due to its high fiber, protein, and antioxidant content.</t>
+  </si>
+  <si>
+    <t>Sautéed veggies offer a low-calorie, nutrient-rich option that supports overall health with fiber, vitamins, minerals, and antioxidants.</t>
+  </si>
+  <si>
+    <t>Broccoli beetroot tikki offers benefits such as being rich in fiber for digestive health, providing essential vitamins and minerals for overall well-being, and offering antioxidants for immune support and inflammation reduction.</t>
+  </si>
+  <si>
+    <t>Summer Delight Salad offers a refreshing and nutrient-rich option, providing hydration, vitamins, minerals, and antioxidants to support overall health and well-being.</t>
+  </si>
+  <si>
+    <t>This wholesome bowl offers a balanced blend of fiber-rich oats, protein-packed curd, nutrient-dense seeds and muesli, along with the natural goodness of an apple, providing sustained energy, digestive support, and essential nutrients in one delicious serving.</t>
+  </si>
+  <si>
+    <t>This wholesome bowl offers sustained energy, digestive support, and essential nutrients, promoting overall health and well-being through its blend of fiber-rich oats, protein-packed curd, nutrient-dense seeds and muesli, and the natural goodness of banana.</t>
+  </si>
+  <si>
+    <t>gr</t>
+  </si>
+  <si>
+    <t>This wholesome bowl offers sustained energy, digestive support, and essential nutrients, promoting overall health and well-being through its blend of fiber-rich oats, protein-packed curd, nutrient-dense seeds and muesli, and the natural goodness of grapes and banana.</t>
+  </si>
+  <si>
+    <t>this bowl provides sustained energy, digestive support, and essential nutrients from oats, curd, mixed seeds, muesli, banana, and mango, promoting overall health and well-being.</t>
+  </si>
+  <si>
+    <t>This bowl provides a balanced blend of fiber, vitamins, minerals, and antioxidants from oats, curd, seeds, muesli, banana, and kiwi, promoting digestive health, sustained energy, and overall well-being.</t>
+  </si>
+  <si>
+    <t>This bowl offers a blend of fiber, vitamins, minerals, and antioxidants, promoting digestive health, sustained energy, and overall well-being.</t>
+  </si>
+  <si>
+    <t>This fruit medley of pomegranate, orange, banana, papaya, apple, and kiwi offers a wealth of vitamins, minerals, antioxidants, and fiber, promoting immune health, digestion, and overall well-being, while providing a delicious and refreshing way to enjoy a variety of nutrients in one bowl.</t>
+  </si>
+  <si>
+    <t>This fruit blend supports heart health with its abundance of fiber, antioxidants, and potassium, which collectively help manage cholesterol, reduce inflammation, and maintain healthy blood pressure levels.</t>
+  </si>
+  <si>
+    <t>This fruit blend serves as a natural energy booster, providing quick carbohydrates and natural sugars for sustained vitality, along with fiber to prevent energy crashes.</t>
+  </si>
+  <si>
+    <t>This fruit mix promotes blood purification through its rich antioxidant content from pomegranate, papaya, and grapes, along with hydration and fiber support from watermelon, orange, and chikoo, aiding in detoxification and improved circulation.</t>
+  </si>
+  <si>
+    <t>This fruit mix enhances skin glow with its hydrating properties, vitamins, and antioxidants from watermelon, orange, pomegranate, pineapple, and avocado, promoting a radiant complexion.</t>
+  </si>
+  <si>
+    <t>This fruit mix aids in detoxification through its fiber and antioxidant-rich composition, supporting digestion and cleansing processes for overall rejuvenation.</t>
+  </si>
+  <si>
+    <t>c("oats","curd","mixed seeds","muesli","banana","grapes")</t>
+  </si>
+  <si>
+    <t>c("oats","curd","mixed seeds","muesli","banana")</t>
+  </si>
+  <si>
+    <t>c("Pomogranate"," Orange","Banana","Grapes","Pineapple")</t>
+  </si>
+  <si>
+    <t>c("oats"," curd","mixed seeds","muesli","banana","mango")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("oats","curd","mixed seeds","muesli","banana"," kiwi") </t>
+  </si>
+  <si>
+    <t>c("oats","curd","mixed seeds","muesli"," Sapodilla")</t>
+  </si>
+  <si>
+    <t>c("oats","curd","mixed seeds","muesli","apple")</t>
+  </si>
+  <si>
+    <t>c("broccoli","cucumber","carrot","lettuce","panner","peanuts","soya","sweet corn")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("cucumber","sesame seed","olive oil","salt","pepper","paneer","carrot","sweet corn","lettuce, lemon") </t>
+  </si>
+  <si>
+    <t>Energy Booster ( E)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,6 +943,31 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -631,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -642,6 +1022,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,31 +1305,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.84375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.07421875" customWidth="1"/>
+    <col min="7" max="7" width="8.15234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.69140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
-    <col min="16" max="16" width="29.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.3828125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.3046875" customWidth="1"/>
+    <col min="16" max="16" width="29.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -995,7 +1379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>38</v>
       </c>
@@ -1045,7 +1429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>41</v>
       </c>
@@ -1095,7 +1479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>42</v>
       </c>
@@ -1145,7 +1529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>45</v>
       </c>
@@ -1195,7 +1579,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>46</v>
       </c>
@@ -1245,7 +1629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>47</v>
       </c>
@@ -1295,7 +1679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>50</v>
       </c>
@@ -1345,7 +1729,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>51</v>
       </c>
@@ -1395,7 +1779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>52</v>
       </c>
@@ -1445,7 +1829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>55</v>
       </c>
@@ -1495,7 +1879,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>56</v>
       </c>
@@ -1545,7 +1929,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>57</v>
       </c>
@@ -1595,7 +1979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>58</v>
       </c>
@@ -1645,7 +2029,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>59</v>
       </c>
@@ -1695,7 +2079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>60</v>
       </c>
@@ -1745,7 +2129,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>62</v>
       </c>
@@ -1795,7 +2179,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>63</v>
       </c>
@@ -1845,7 +2229,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>64</v>
       </c>
@@ -1895,7 +2279,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>68</v>
       </c>
@@ -1945,7 +2329,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>69</v>
       </c>
@@ -1995,7 +2379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>72</v>
       </c>
@@ -2045,7 +2429,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>74</v>
       </c>
@@ -2095,7 +2479,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>75</v>
       </c>
@@ -2145,7 +2529,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>78</v>
       </c>
@@ -2195,7 +2579,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4">
         <v>79</v>
       </c>
@@ -2245,7 +2629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>82</v>
       </c>
@@ -2295,7 +2679,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>83</v>
       </c>
@@ -2345,7 +2729,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>84</v>
       </c>
@@ -2395,7 +2779,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>85</v>
       </c>
@@ -2445,7 +2829,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>86</v>
       </c>
@@ -2495,7 +2879,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>87</v>
       </c>
@@ -2545,7 +2929,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>92</v>
       </c>
@@ -2595,7 +2979,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>93</v>
       </c>
@@ -2645,7 +3029,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>94</v>
       </c>
@@ -2695,7 +3079,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>97</v>
       </c>
@@ -2745,7 +3129,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>101</v>
       </c>
@@ -2795,7 +3179,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>102</v>
       </c>
@@ -2845,7 +3229,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4">
         <v>104</v>
       </c>
@@ -2895,7 +3279,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4">
         <v>105</v>
       </c>
@@ -2945,7 +3329,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="4">
         <v>110</v>
       </c>
@@ -2995,7 +3379,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>112</v>
       </c>
@@ -3045,7 +3429,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="4">
         <v>113</v>
       </c>
@@ -3095,7 +3479,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>114</v>
       </c>
@@ -3145,7 +3529,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>115</v>
       </c>
@@ -3195,7 +3579,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>116</v>
       </c>
@@ -3245,7 +3629,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>117</v>
       </c>
@@ -3295,7 +3679,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>118</v>
       </c>
@@ -3345,7 +3729,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>119</v>
       </c>
@@ -3395,7 +3779,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="4">
         <v>121</v>
       </c>
@@ -3445,7 +3829,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>123</v>
       </c>
@@ -3493,6 +3877,1959 @@
       </c>
       <c r="P51" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>124</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52">
+        <v>60</v>
+      </c>
+      <c r="D52">
+        <v>30</v>
+      </c>
+      <c r="E52">
+        <v>90</v>
+      </c>
+      <c r="F52" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52">
+        <v>109</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>101.4</v>
+      </c>
+      <c r="M52">
+        <v>13.8</v>
+      </c>
+      <c r="N52">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="O52">
+        <v>14.4</v>
+      </c>
+      <c r="P52" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>125</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53">
+        <v>50</v>
+      </c>
+      <c r="D53">
+        <v>45</v>
+      </c>
+      <c r="E53">
+        <v>95</v>
+      </c>
+      <c r="F53" t="s">
+        <v>173</v>
+      </c>
+      <c r="G53">
+        <v>384</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>95</v>
+      </c>
+      <c r="M53">
+        <v>21</v>
+      </c>
+      <c r="N53">
+        <v>64.3</v>
+      </c>
+      <c r="O53">
+        <v>6.5</v>
+      </c>
+      <c r="P53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>126</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54">
+        <v>60</v>
+      </c>
+      <c r="D54">
+        <v>50</v>
+      </c>
+      <c r="E54">
+        <v>110</v>
+      </c>
+      <c r="F54" t="s">
+        <v>174</v>
+      </c>
+      <c r="G54">
+        <v>365</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>117</v>
+      </c>
+      <c r="M54">
+        <v>11</v>
+      </c>
+      <c r="N54">
+        <v>67</v>
+      </c>
+      <c r="O54">
+        <v>8.6</v>
+      </c>
+      <c r="P54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>127</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C55">
+        <v>55</v>
+      </c>
+      <c r="D55">
+        <v>40</v>
+      </c>
+      <c r="E55">
+        <v>95</v>
+      </c>
+      <c r="F55" t="s">
+        <v>175</v>
+      </c>
+      <c r="G55">
+        <v>276</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>2</v>
+      </c>
+      <c r="L55">
+        <v>69</v>
+      </c>
+      <c r="M55">
+        <v>11.4</v>
+      </c>
+      <c r="N55">
+        <v>47</v>
+      </c>
+      <c r="O55">
+        <v>2.7</v>
+      </c>
+      <c r="P55" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>128</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56">
+        <v>45</v>
+      </c>
+      <c r="D56">
+        <v>30</v>
+      </c>
+      <c r="E56">
+        <v>75</v>
+      </c>
+      <c r="F56" t="s">
+        <v>176</v>
+      </c>
+      <c r="G56">
+        <v>344</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>96</v>
+      </c>
+      <c r="M56">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="N56">
+        <v>52</v>
+      </c>
+      <c r="O56">
+        <v>7.7</v>
+      </c>
+      <c r="P56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>129</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C57">
+        <v>45</v>
+      </c>
+      <c r="D57">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>75</v>
+      </c>
+      <c r="F57" t="s">
+        <v>180</v>
+      </c>
+      <c r="G57">
+        <v>220.1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>81.59</v>
+      </c>
+      <c r="M57">
+        <v>11.85</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>10.58</v>
+      </c>
+      <c r="P57" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>130</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58">
+        <v>30</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+      <c r="E58">
+        <v>50</v>
+      </c>
+      <c r="F58" t="s">
+        <v>187</v>
+      </c>
+      <c r="G58">
+        <v>8.75</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1.25</v>
+      </c>
+      <c r="M58">
+        <v>0.875</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>1.125</v>
+      </c>
+      <c r="P58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>131</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59">
+        <v>30</v>
+      </c>
+      <c r="D59">
+        <v>30</v>
+      </c>
+      <c r="E59">
+        <v>60</v>
+      </c>
+      <c r="F59" t="s">
+        <v>188</v>
+      </c>
+      <c r="G59">
+        <v>123</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>2</v>
+      </c>
+      <c r="L59">
+        <v>30</v>
+      </c>
+      <c r="M59">
+        <v>8.4</v>
+      </c>
+      <c r="N59">
+        <v>15</v>
+      </c>
+      <c r="O59">
+        <v>2.7</v>
+      </c>
+      <c r="P59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>132</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60">
+        <v>45</v>
+      </c>
+      <c r="D60">
+        <v>35</v>
+      </c>
+      <c r="E60">
+        <v>80</v>
+      </c>
+      <c r="F60" t="s">
+        <v>189</v>
+      </c>
+      <c r="G60">
+        <v>45</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M60">
+        <v>1.5</v>
+      </c>
+      <c r="N60">
+        <v>4.5</v>
+      </c>
+      <c r="O60">
+        <v>1.8</v>
+      </c>
+      <c r="P60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>133</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61">
+        <v>30</v>
+      </c>
+      <c r="D61">
+        <v>20</v>
+      </c>
+      <c r="E61">
+        <v>50</v>
+      </c>
+      <c r="F61" t="s">
+        <v>190</v>
+      </c>
+      <c r="G61">
+        <v>46</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>10.96</v>
+      </c>
+      <c r="M61">
+        <v>1.73</v>
+      </c>
+      <c r="N61">
+        <v>5.19</v>
+      </c>
+      <c r="O61">
+        <v>2.31</v>
+      </c>
+      <c r="P61" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>134</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <v>30</v>
+      </c>
+      <c r="E62">
+        <v>50</v>
+      </c>
+      <c r="F62" t="s">
+        <v>191</v>
+      </c>
+      <c r="G62">
+        <v>36.24</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="M62">
+        <v>3.02</v>
+      </c>
+      <c r="N62">
+        <v>6.04</v>
+      </c>
+      <c r="O62">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="P62" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>135</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63">
+        <v>45</v>
+      </c>
+      <c r="D63">
+        <v>30</v>
+      </c>
+      <c r="E63">
+        <v>75</v>
+      </c>
+      <c r="F63" t="s">
+        <v>192</v>
+      </c>
+      <c r="G63">
+        <v>74.16</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="M63">
+        <v>6.74</v>
+      </c>
+      <c r="N63">
+        <v>5.76</v>
+      </c>
+      <c r="O63">
+        <v>3.37</v>
+      </c>
+      <c r="P63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>136</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64">
+        <v>30</v>
+      </c>
+      <c r="D64">
+        <v>20</v>
+      </c>
+      <c r="E64">
+        <v>50</v>
+      </c>
+      <c r="F64" t="s">
+        <v>243</v>
+      </c>
+      <c r="G64">
+        <v>100.9</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>22.14</v>
+      </c>
+      <c r="M64">
+        <v>10.02</v>
+      </c>
+      <c r="N64">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="O64">
+        <v>5.5</v>
+      </c>
+      <c r="P64" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>137</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C65">
+        <v>30</v>
+      </c>
+      <c r="D65">
+        <v>35</v>
+      </c>
+      <c r="E65">
+        <v>65</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G65">
+        <v>220</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0.1</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>21.8</v>
+      </c>
+      <c r="M65">
+        <v>12</v>
+      </c>
+      <c r="N65">
+        <v>9.6</v>
+      </c>
+      <c r="O65">
+        <v>6.7</v>
+      </c>
+      <c r="P65" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>138</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66">
+        <v>30</v>
+      </c>
+      <c r="D66">
+        <v>35</v>
+      </c>
+      <c r="E66">
+        <v>65</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G66">
+        <v>250.5</v>
+      </c>
+      <c r="H66">
+        <v>0.1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>0.2</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>60</v>
+      </c>
+      <c r="M66">
+        <v>12</v>
+      </c>
+      <c r="N66">
+        <v>34.5</v>
+      </c>
+      <c r="O66">
+        <v>4.5</v>
+      </c>
+      <c r="P66" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>139</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C67">
+        <v>30</v>
+      </c>
+      <c r="D67">
+        <v>35</v>
+      </c>
+      <c r="E67">
+        <v>65</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G67">
+        <v>230.6</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>5</v>
+      </c>
+      <c r="L67">
+        <v>50</v>
+      </c>
+      <c r="M67">
+        <v>13</v>
+      </c>
+      <c r="N67">
+        <v>45</v>
+      </c>
+      <c r="O67">
+        <v>4.5</v>
+      </c>
+      <c r="P67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="68" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>140</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68">
+        <v>30</v>
+      </c>
+      <c r="D68">
+        <v>35</v>
+      </c>
+      <c r="E68">
+        <v>65</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="G68">
+        <v>240.8</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>5.5</v>
+      </c>
+      <c r="L68">
+        <v>65</v>
+      </c>
+      <c r="M68">
+        <v>14</v>
+      </c>
+      <c r="N68">
+        <v>43.4</v>
+      </c>
+      <c r="O68">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P68" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="69" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>141</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69">
+        <v>30</v>
+      </c>
+      <c r="D69">
+        <v>35</v>
+      </c>
+      <c r="E69">
+        <v>65</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="G69">
+        <v>195.8</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>4.2</v>
+      </c>
+      <c r="L69">
+        <v>45.5</v>
+      </c>
+      <c r="M69">
+        <v>13.5</v>
+      </c>
+      <c r="N69">
+        <v>37.5</v>
+      </c>
+      <c r="O69">
+        <v>2.1</v>
+      </c>
+      <c r="P69" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>142</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70">
+        <v>30</v>
+      </c>
+      <c r="D70">
+        <v>35</v>
+      </c>
+      <c r="E70">
+        <v>65</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="G70">
+        <v>220.4</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>5.3</v>
+      </c>
+      <c r="L70">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="M70">
+        <v>12.3</v>
+      </c>
+      <c r="N70">
+        <v>49.5</v>
+      </c>
+      <c r="O70">
+        <v>1.2</v>
+      </c>
+      <c r="P70" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>143</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71">
+        <v>30</v>
+      </c>
+      <c r="D71">
+        <v>25</v>
+      </c>
+      <c r="E71">
+        <v>55</v>
+      </c>
+      <c r="F71" t="s">
+        <v>275</v>
+      </c>
+      <c r="G71">
+        <v>300</v>
+      </c>
+      <c r="H71">
+        <v>9</v>
+      </c>
+      <c r="I71">
+        <v>3</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>60</v>
+      </c>
+      <c r="L71">
+        <v>10</v>
+      </c>
+      <c r="M71">
+        <v>15</v>
+      </c>
+      <c r="N71">
+        <v>10</v>
+      </c>
+      <c r="O71">
+        <v>12</v>
+      </c>
+      <c r="P71" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>144</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72">
+        <v>35</v>
+      </c>
+      <c r="D72">
+        <v>25</v>
+      </c>
+      <c r="E72">
+        <v>60</v>
+      </c>
+      <c r="F72" t="s">
+        <v>274</v>
+      </c>
+      <c r="G72">
+        <v>350</v>
+      </c>
+      <c r="H72">
+        <v>8</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>50</v>
+      </c>
+      <c r="L72">
+        <v>8</v>
+      </c>
+      <c r="M72">
+        <v>10</v>
+      </c>
+      <c r="N72">
+        <v>12</v>
+      </c>
+      <c r="O72">
+        <v>15</v>
+      </c>
+      <c r="P72" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ72" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="73" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>145</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C73">
+        <v>40</v>
+      </c>
+      <c r="D73">
+        <v>25</v>
+      </c>
+      <c r="E73">
+        <v>65</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="G73">
+        <v>300</v>
+      </c>
+      <c r="H73">
+        <v>9</v>
+      </c>
+      <c r="I73">
+        <v>3</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>60</v>
+      </c>
+      <c r="L73">
+        <v>10</v>
+      </c>
+      <c r="M73">
+        <v>15</v>
+      </c>
+      <c r="N73">
+        <v>10</v>
+      </c>
+      <c r="O73">
+        <v>9</v>
+      </c>
+      <c r="P73" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>146</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C74">
+        <v>30</v>
+      </c>
+      <c r="D74">
+        <v>20</v>
+      </c>
+      <c r="E74">
+        <v>50</v>
+      </c>
+      <c r="F74" t="s">
+        <v>278</v>
+      </c>
+      <c r="G74">
+        <v>390.8</v>
+      </c>
+      <c r="H74">
+        <v>8</v>
+      </c>
+      <c r="I74">
+        <v>3</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>70</v>
+      </c>
+      <c r="L74">
+        <v>10</v>
+      </c>
+      <c r="M74">
+        <v>23.9</v>
+      </c>
+      <c r="N74">
+        <v>9.1</v>
+      </c>
+      <c r="O74">
+        <v>13</v>
+      </c>
+      <c r="P74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:36" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>147</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C75">
+        <v>40</v>
+      </c>
+      <c r="D75">
+        <v>30</v>
+      </c>
+      <c r="E75">
+        <v>70</v>
+      </c>
+      <c r="F75" t="s">
+        <v>279</v>
+      </c>
+      <c r="G75" s="6">
+        <v>370</v>
+      </c>
+      <c r="H75">
+        <v>9.5</v>
+      </c>
+      <c r="I75">
+        <v>3.9</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>30</v>
+      </c>
+      <c r="L75">
+        <v>9.5</v>
+      </c>
+      <c r="M75">
+        <v>22.3</v>
+      </c>
+      <c r="N75">
+        <v>10.8</v>
+      </c>
+      <c r="O75">
+        <v>11</v>
+      </c>
+      <c r="P75" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="76" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>148</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C76">
+        <v>35</v>
+      </c>
+      <c r="D76">
+        <v>35</v>
+      </c>
+      <c r="E76">
+        <v>70</v>
+      </c>
+      <c r="F76" t="s">
+        <v>280</v>
+      </c>
+      <c r="G76">
+        <v>300</v>
+      </c>
+      <c r="H76">
+        <v>7</v>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76">
+        <v>10</v>
+      </c>
+      <c r="K76">
+        <v>60</v>
+      </c>
+      <c r="L76">
+        <v>55</v>
+      </c>
+      <c r="M76">
+        <v>10</v>
+      </c>
+      <c r="N76">
+        <v>20</v>
+      </c>
+      <c r="O76">
+        <v>12</v>
+      </c>
+      <c r="P76" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>149</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C77">
+        <v>40</v>
+      </c>
+      <c r="D77">
+        <v>45</v>
+      </c>
+      <c r="E77">
+        <v>95</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G77">
+        <v>220</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>25</v>
+      </c>
+      <c r="L77">
+        <v>35</v>
+      </c>
+      <c r="M77">
+        <v>5</v>
+      </c>
+      <c r="N77">
+        <v>30</v>
+      </c>
+      <c r="O77">
+        <v>4</v>
+      </c>
+      <c r="P77" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>150</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C78">
+        <v>40</v>
+      </c>
+      <c r="D78">
+        <v>45</v>
+      </c>
+      <c r="E78">
+        <v>95</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="G78">
+        <v>400.1</v>
+      </c>
+      <c r="H78">
+        <v>25</v>
+      </c>
+      <c r="I78">
+        <v>5</v>
+      </c>
+      <c r="J78">
+        <v>5</v>
+      </c>
+      <c r="K78">
+        <v>200.2</v>
+      </c>
+      <c r="L78">
+        <v>45</v>
+      </c>
+      <c r="M78">
+        <v>8</v>
+      </c>
+      <c r="N78">
+        <v>30</v>
+      </c>
+      <c r="O78">
+        <v>15.5</v>
+      </c>
+      <c r="P78" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>151</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79">
+        <v>30</v>
+      </c>
+      <c r="D79">
+        <v>35</v>
+      </c>
+      <c r="E79">
+        <v>65</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G79">
+        <v>200</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>40</v>
+      </c>
+      <c r="L79">
+        <v>35</v>
+      </c>
+      <c r="M79">
+        <v>5</v>
+      </c>
+      <c r="N79">
+        <v>35</v>
+      </c>
+      <c r="O79">
+        <v>2</v>
+      </c>
+      <c r="P79" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="80" spans="1:36" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>152</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80">
+        <v>40</v>
+      </c>
+      <c r="D80">
+        <v>45</v>
+      </c>
+      <c r="E80">
+        <v>85</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="G80">
+        <v>180</v>
+      </c>
+      <c r="H80">
+        <v>3</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>60.5</v>
+      </c>
+      <c r="L80">
+        <v>25</v>
+      </c>
+      <c r="M80">
+        <v>6</v>
+      </c>
+      <c r="N80">
+        <v>15</v>
+      </c>
+      <c r="O80">
+        <v>7</v>
+      </c>
+      <c r="P80" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>153</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C81">
+        <v>50</v>
+      </c>
+      <c r="D81">
+        <v>40</v>
+      </c>
+      <c r="E81">
+        <v>90</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="G81">
+        <v>250.4</v>
+      </c>
+      <c r="H81">
+        <v>4</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>5</v>
+      </c>
+      <c r="K81">
+        <v>100</v>
+      </c>
+      <c r="L81">
+        <v>35.1</v>
+      </c>
+      <c r="M81">
+        <v>7</v>
+      </c>
+      <c r="N81">
+        <v>15</v>
+      </c>
+      <c r="O81">
+        <v>8</v>
+      </c>
+      <c r="P81" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>154</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82">
+        <v>50</v>
+      </c>
+      <c r="D82">
+        <v>30</v>
+      </c>
+      <c r="E82">
+        <v>80</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="G82">
+        <v>260</v>
+      </c>
+      <c r="H82">
+        <v>5</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>5</v>
+      </c>
+      <c r="K82">
+        <v>100</v>
+      </c>
+      <c r="L82">
+        <v>45</v>
+      </c>
+      <c r="M82">
+        <v>6</v>
+      </c>
+      <c r="N82">
+        <v>30</v>
+      </c>
+      <c r="O82">
+        <v>9</v>
+      </c>
+      <c r="P82" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>155</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C83">
+        <v>50</v>
+      </c>
+      <c r="D83">
+        <v>60</v>
+      </c>
+      <c r="E83">
+        <v>110</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G83">
+        <v>350</v>
+      </c>
+      <c r="H83">
+        <v>20</v>
+      </c>
+      <c r="I83">
+        <v>7</v>
+      </c>
+      <c r="J83">
+        <v>20</v>
+      </c>
+      <c r="K83">
+        <v>400</v>
+      </c>
+      <c r="L83">
+        <v>30</v>
+      </c>
+      <c r="M83">
+        <v>12.1</v>
+      </c>
+      <c r="N83">
+        <v>10</v>
+      </c>
+      <c r="O83">
+        <v>18</v>
+      </c>
+      <c r="P83" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>156</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C84">
+        <v>30</v>
+      </c>
+      <c r="D84">
+        <v>50</v>
+      </c>
+      <c r="E84">
+        <v>80</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="G84">
+        <v>350</v>
+      </c>
+      <c r="H84">
+        <v>15</v>
+      </c>
+      <c r="I84">
+        <v>3.4</v>
+      </c>
+      <c r="J84">
+        <v>5</v>
+      </c>
+      <c r="K84">
+        <v>200</v>
+      </c>
+      <c r="L84">
+        <v>20</v>
+      </c>
+      <c r="M84">
+        <v>8</v>
+      </c>
+      <c r="N84">
+        <v>7</v>
+      </c>
+      <c r="O84">
+        <v>20</v>
+      </c>
+      <c r="P84" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>157</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C85">
+        <v>50</v>
+      </c>
+      <c r="D85">
+        <v>50</v>
+      </c>
+      <c r="E85">
+        <v>100</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="G85">
+        <v>200</v>
+      </c>
+      <c r="H85">
+        <v>4</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>5</v>
+      </c>
+      <c r="K85">
+        <v>100.2</v>
+      </c>
+      <c r="L85">
+        <v>45</v>
+      </c>
+      <c r="M85">
+        <v>5</v>
+      </c>
+      <c r="N85">
+        <v>30</v>
+      </c>
+      <c r="O85">
+        <v>7.5</v>
+      </c>
+      <c r="P85" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>158</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C86">
+        <v>40</v>
+      </c>
+      <c r="D86">
+        <v>45</v>
+      </c>
+      <c r="E86">
+        <v>85</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="G86">
+        <v>200</v>
+      </c>
+      <c r="H86">
+        <v>10</v>
+      </c>
+      <c r="I86">
+        <v>3.4</v>
+      </c>
+      <c r="J86">
+        <v>5</v>
+      </c>
+      <c r="K86">
+        <v>150</v>
+      </c>
+      <c r="L86">
+        <v>25</v>
+      </c>
+      <c r="M86">
+        <v>6</v>
+      </c>
+      <c r="N86">
+        <v>10</v>
+      </c>
+      <c r="O86">
+        <v>6</v>
+      </c>
+      <c r="P86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>159</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C87">
+        <v>45</v>
+      </c>
+      <c r="D87">
+        <v>45</v>
+      </c>
+      <c r="E87">
+        <v>85</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G87">
+        <v>180</v>
+      </c>
+      <c r="H87">
+        <v>3</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>250</v>
+      </c>
+      <c r="L87">
+        <v>30.3</v>
+      </c>
+      <c r="M87">
+        <v>8</v>
+      </c>
+      <c r="N87">
+        <v>5</v>
+      </c>
+      <c r="O87">
+        <v>12</v>
+      </c>
+      <c r="P87" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>160</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C88">
+        <v>50</v>
+      </c>
+      <c r="D88">
+        <v>50</v>
+      </c>
+      <c r="E88">
+        <v>100</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G88">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="H88">
+        <v>10</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>300</v>
+      </c>
+      <c r="L88">
+        <v>20</v>
+      </c>
+      <c r="M88">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N88">
+        <v>8</v>
+      </c>
+      <c r="O88">
+        <v>5</v>
+      </c>
+      <c r="P88" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>161</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C89">
+        <v>35</v>
+      </c>
+      <c r="D89">
+        <v>50</v>
+      </c>
+      <c r="E89">
+        <v>85</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G89">
+        <v>300</v>
+      </c>
+      <c r="H89">
+        <v>15</v>
+      </c>
+      <c r="I89">
+        <v>3</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>400</v>
+      </c>
+      <c r="L89">
+        <v>30</v>
+      </c>
+      <c r="M89">
+        <v>8</v>
+      </c>
+      <c r="N89">
+        <v>5</v>
+      </c>
+      <c r="O89">
+        <v>6</v>
+      </c>
+      <c r="P89" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>162</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90">
+        <v>30</v>
+      </c>
+      <c r="D90">
+        <v>55</v>
+      </c>
+      <c r="E90">
+        <v>85</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="G90">
+        <v>250</v>
+      </c>
+      <c r="H90">
+        <v>10</v>
+      </c>
+      <c r="I90">
+        <v>3</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>300.3</v>
+      </c>
+      <c r="L90">
+        <v>30</v>
+      </c>
+      <c r="M90">
+        <v>7</v>
+      </c>
+      <c r="N90">
+        <v>10.1</v>
+      </c>
+      <c r="O90">
+        <v>8.5</v>
+      </c>
+      <c r="P90" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>